<commit_message>
Rev D of audio spectrum board
</commit_message>
<xml_diff>
--- a/modules/audio_spectrum/rev_d/audio_spectrum_bom.xlsx
+++ b/modules/audio_spectrum/rev_d/audio_spectrum_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="audio_spectrum_bom" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="179">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -52,24 +52,30 @@
     <t xml:space="preserve">8pF</t>
   </si>
   <si>
+    <t xml:space="preserve">CAPACITOR0402_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402 Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-8230-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2nF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAPACITOR0603_CAP</t>
   </si>
   <si>
     <t xml:space="preserve">0603_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402 Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">478-1215-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2nF</t>
-  </si>
-  <si>
     <t xml:space="preserve">C12, C13</t>
   </si>
   <si>
@@ -100,12 +106,6 @@
     <t xml:space="preserve">C20, C21, C22, C23</t>
   </si>
   <si>
-    <t xml:space="preserve">CAPACITOR0402_CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402_CAP</t>
-  </si>
-  <si>
     <t xml:space="preserve">C24</t>
   </si>
   <si>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C25, C26, C27</t>
+    <t xml:space="preserve">C25, C26, C27, C33, C34</t>
   </si>
   <si>
     <t xml:space="preserve">490-1536-1-ND</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">1.5k</t>
   </si>
   <si>
-    <t xml:space="preserve">FERRITE_BEAD0603</t>
+    <t xml:space="preserve">FERRITE_BEAD0402</t>
   </si>
   <si>
     <t xml:space="preserve">FB1</t>
@@ -274,21 +274,21 @@
     <t xml:space="preserve">LED-0603</t>
   </si>
   <si>
+    <t xml:space="preserve">LED0, LED2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160-1447-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED1, LED3</t>
   </si>
   <si>
-    <t xml:space="preserve">LED</t>
-  </si>
-  <si>
     <t xml:space="preserve">160-1446-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">LED2, LED4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">160-1447-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">4k-200k</t>
   </si>
   <si>
@@ -370,7 +370,7 @@
     <t xml:space="preserve">20k</t>
   </si>
   <si>
-    <t xml:space="preserve">R17, R18, R19, R20</t>
+    <t xml:space="preserve">R17, R18, R19, R20, R32, R33, R34, R35</t>
   </si>
   <si>
     <t xml:space="preserve">RHM20KCGCT-ND</t>
@@ -452,21 +452,6 @@
   </si>
   <si>
     <t xml:space="preserve">SW1020CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST_POINT_0.040IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTPOINT_0.040IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.040in Test Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5001K-ND</t>
   </si>
   <si>
     <t xml:space="preserve">AT45DB641EUDFN</t>
@@ -586,7 +571,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -668,22 +652,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.9540816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="25.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.5102040816326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.4234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.51530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,7 +701,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
@@ -740,108 +724,108 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>28</v>
@@ -855,16 +839,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>31</v>
@@ -878,16 +862,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>34</v>
@@ -907,10 +891,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>36</v>
@@ -924,16 +908,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>39</v>
@@ -947,16 +931,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>42</v>
@@ -976,10 +960,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>45</v>
@@ -993,16 +977,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>48</v>
@@ -1022,10 +1006,10 @@
         <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>51</v>
@@ -1039,16 +1023,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>54</v>
@@ -1062,7 +1046,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>56</v>
@@ -1082,7 +1066,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>60</v>
@@ -1105,7 +1089,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>64</v>
@@ -1145,7 +1129,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>71</v>
@@ -1168,7 +1152,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>77</v>
@@ -1191,7 +1175,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>82</v>
@@ -1214,7 +1198,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>82</v>
@@ -1237,7 +1221,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>89</v>
@@ -1260,7 +1244,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>95</v>
@@ -1289,7 +1273,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -1312,7 +1296,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>107</v>
@@ -1381,7 +1365,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>115</v>
@@ -1450,7 +1434,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>124</v>
@@ -1473,7 +1457,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>127</v>
@@ -1496,7 +1480,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>118</v>
@@ -1542,7 +1526,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>135</v>
@@ -1565,7 +1549,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>56</v>
@@ -1634,7 +1618,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>149</v>
@@ -1657,7 +1641,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>154</v>
@@ -1666,27 +1650,27 @@
         <v>154</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="F43" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="G43" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>159</v>
@@ -1703,7 +1687,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>163</v>
@@ -1749,48 +1733,25 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>173</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B48" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>